<commit_message>
New version of Similarity spreadsheet Syllabus to Course catalog, Syllabus to Outcomes, Total
New version of Similarity spreadsheet Syllabus to Course catalog, Syllabus to Outcomes, Total
</commit_message>
<xml_diff>
--- a/SRP Similarity.xlsx
+++ b/SRP Similarity.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Course Catalog</t>
   </si>
@@ -78,6 +78,18 @@
   </si>
   <si>
     <t>CS205</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>Syllabus to Course Catalog</t>
+  </si>
+  <si>
+    <t>Syllabus to ABET Outcomes</t>
+  </si>
+  <si>
+    <t>Total Similarity</t>
   </si>
 </sst>
 </file>
@@ -177,17 +189,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Measure of Similarity</a:t>
+              <a:t>Measure</a:t>
             </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Catalog vs Syllabus</a:t>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of Similarity</a:t>
             </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -229,8 +237,149 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Similarity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$12:$B$14</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>CS310</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CS205</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CS104</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$12:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7645-46E6-80B6-264839C30373}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Syllabus to ABET Outcomes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$12:$B$14</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>CS310</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CS205</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CS104</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$12:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7645-46E6-80B6-264839C30373}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Syllabus to Course Catalog</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -247,13 +396,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
+                  <c:v>CS310</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CS205</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>CS104</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>CS310</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>CS205</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -278,7 +427,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9C1F-473F-B391-33D88050F896}"/>
+              <c16:uniqueId val="{00000000-7645-46E6-80B6-264839C30373}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -291,16 +440,30 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="443516632"/>
-        <c:axId val="443510728"/>
+        <c:axId val="453609160"/>
+        <c:axId val="453611128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="443516632"/>
+        <c:axId val="453609160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -338,7 +501,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443510728"/>
+        <c:crossAx val="453611128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -346,7 +509,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="443510728"/>
+        <c:axId val="453611128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -397,7 +560,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443516632"/>
+        <c:crossAx val="453609160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -409,6 +572,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -995,20 +1190,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>280987</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>585787</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1291,8 +1486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1552,28 +1747,63 @@
       </c>
       <c r="P10" s="1"/>
     </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C12">
         <v>2</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <f>C12+D12</f>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13">
         <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ref="E13:E14" si="4">C13+D13</f>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C14">
         <v>3.5</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="4"/>
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>